<commit_message>
refs #489 Formatierung angepasst
</commit_message>
<xml_diff>
--- a/doc/03_Technischer_Bericht_Teil_2/05_Projektmanagement/03 _Risikomanagement.xlsx
+++ b/doc/03_Technischer_Bericht_Teil_2/05_Projektmanagement/03 _Risikomanagement.xlsx
@@ -638,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -795,9 +795,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -843,6 +840,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -855,20 +870,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -885,18 +894,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -947,7 +944,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -966,9 +963,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1006,7 +1003,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1078,7 +1075,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1256,10 +1253,10 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B8" sqref="B8:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
@@ -1288,11 +1285,11 @@
         <v>38</v>
       </c>
       <c r="B5" s="59"/>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="82"/>
-      <c r="E5" s="83"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="78"/>
     </row>
     <row r="6" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
@@ -1305,10 +1302,10 @@
       <c r="A7" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="85"/>
+      <c r="C7" s="80"/>
       <c r="D7" s="60" t="s">
         <v>48</v>
       </c>
@@ -1320,10 +1317,10 @@
       <c r="A8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="90" t="s">
+      <c r="B8" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="91"/>
+      <c r="C8" s="94"/>
       <c r="D8" s="28" t="s">
         <v>24</v>
       </c>
@@ -1333,10 +1330,10 @@
       <c r="A9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="88" t="s">
+      <c r="B9" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="89"/>
+      <c r="C9" s="92"/>
       <c r="D9" s="29" t="s">
         <v>24</v>
       </c>
@@ -1346,10 +1343,10 @@
       <c r="A10" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="89"/>
+      <c r="C10" s="92"/>
       <c r="D10" s="29" t="s">
         <v>24</v>
       </c>
@@ -1359,10 +1356,10 @@
       <c r="A11" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="89"/>
+      <c r="C11" s="92"/>
       <c r="D11" s="29"/>
       <c r="E11" s="27" t="s">
         <v>24</v>
@@ -1370,8 +1367,8 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
-      <c r="B12" s="92"/>
-      <c r="C12" s="93"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="88"/>
       <c r="D12" s="31"/>
       <c r="E12" s="32"/>
       <c r="H12" s="3"/>
@@ -1381,8 +1378,8 @@
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="89"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1394,11 +1391,11 @@
         <v>39</v>
       </c>
       <c r="B14" s="59"/>
-      <c r="C14" s="82" t="s">
+      <c r="C14" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="82"/>
-      <c r="E14" s="83"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="78"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -1421,10 +1418,10 @@
       <c r="A16" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="84" t="s">
+      <c r="B16" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="85"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="60" t="s">
         <v>48</v>
       </c>
@@ -1439,8 +1436,8 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
-      <c r="B17" s="86"/>
-      <c r="C17" s="87"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="90"/>
       <c r="D17" s="28"/>
       <c r="E17" s="19"/>
       <c r="H17" s="3"/>
@@ -1451,8 +1448,8 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
-      <c r="B18" s="78"/>
-      <c r="C18" s="79"/>
+      <c r="B18" s="83"/>
+      <c r="C18" s="84"/>
       <c r="D18" s="29"/>
       <c r="E18" s="27"/>
       <c r="H18" s="3"/>
@@ -1463,8 +1460,8 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
-      <c r="B19" s="78"/>
-      <c r="C19" s="79"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="84"/>
       <c r="D19" s="29"/>
       <c r="E19" s="27"/>
       <c r="H19" s="3"/>
@@ -1475,8 +1472,8 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
-      <c r="B20" s="78"/>
-      <c r="C20" s="79"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="84"/>
       <c r="D20" s="29"/>
       <c r="E20" s="27"/>
       <c r="H20" s="3"/>
@@ -1487,8 +1484,8 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
-      <c r="B21" s="80"/>
-      <c r="C21" s="81"/>
+      <c r="B21" s="85"/>
+      <c r="C21" s="86"/>
       <c r="D21" s="30"/>
       <c r="E21" s="20"/>
     </row>
@@ -1498,11 +1495,11 @@
         <v>40</v>
       </c>
       <c r="B23" s="59"/>
-      <c r="C23" s="82" t="s">
+      <c r="C23" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="82"/>
-      <c r="E23" s="83"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="78"/>
     </row>
     <row r="24" spans="1:12" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
@@ -1515,10 +1512,10 @@
       <c r="A25" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="84" t="s">
+      <c r="B25" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="85"/>
+      <c r="C25" s="80"/>
       <c r="D25" s="60" t="s">
         <v>48</v>
       </c>
@@ -1528,36 +1525,36 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="17"/>
-      <c r="B26" s="86"/>
-      <c r="C26" s="95"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="82"/>
       <c r="D26" s="28"/>
       <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
-      <c r="B27" s="78"/>
-      <c r="C27" s="79"/>
+      <c r="B27" s="83"/>
+      <c r="C27" s="84"/>
       <c r="D27" s="29"/>
       <c r="E27" s="27"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
-      <c r="B28" s="78"/>
-      <c r="C28" s="79"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="84"/>
       <c r="D28" s="29"/>
       <c r="E28" s="27"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
-      <c r="B29" s="78"/>
-      <c r="C29" s="79"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="84"/>
       <c r="D29" s="29"/>
       <c r="E29" s="27"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
-      <c r="B30" s="80"/>
-      <c r="C30" s="81"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="86"/>
       <c r="D30" s="30"/>
       <c r="E30" s="20"/>
     </row>
@@ -1567,11 +1564,11 @@
         <v>41</v>
       </c>
       <c r="B32" s="59"/>
-      <c r="C32" s="82" t="s">
+      <c r="C32" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="82"/>
-      <c r="E32" s="83"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="78"/>
     </row>
     <row r="33" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15"/>
@@ -1584,10 +1581,10 @@
       <c r="A34" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="84" t="s">
+      <c r="B34" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="85"/>
+      <c r="C34" s="80"/>
       <c r="D34" s="60" t="s">
         <v>48</v>
       </c>
@@ -1597,36 +1594,36 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="17"/>
-      <c r="B35" s="86"/>
-      <c r="C35" s="87"/>
+      <c r="B35" s="81"/>
+      <c r="C35" s="90"/>
       <c r="D35" s="28"/>
       <c r="E35" s="19"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="26"/>
-      <c r="B36" s="78"/>
-      <c r="C36" s="79"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="84"/>
       <c r="D36" s="29"/>
       <c r="E36" s="27"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="26"/>
-      <c r="B37" s="78"/>
-      <c r="C37" s="79"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="84"/>
       <c r="D37" s="29"/>
       <c r="E37" s="27"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="26"/>
-      <c r="B38" s="78"/>
-      <c r="C38" s="79"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="84"/>
       <c r="D38" s="29"/>
       <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
-      <c r="B39" s="80"/>
-      <c r="C39" s="81"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="86"/>
       <c r="D39" s="30"/>
       <c r="E39" s="20"/>
     </row>
@@ -1635,11 +1632,11 @@
         <v>42</v>
       </c>
       <c r="B42" s="59"/>
-      <c r="C42" s="82" t="s">
+      <c r="C42" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="82"/>
-      <c r="E42" s="83"/>
+      <c r="D42" s="77"/>
+      <c r="E42" s="78"/>
     </row>
     <row r="43" spans="1:5" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="15"/>
@@ -1652,10 +1649,10 @@
       <c r="A44" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="84" t="s">
+      <c r="B44" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C44" s="85"/>
+      <c r="C44" s="80"/>
       <c r="D44" s="60" t="s">
         <v>48</v>
       </c>
@@ -1665,48 +1662,54 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
-      <c r="B45" s="86"/>
-      <c r="C45" s="87"/>
+      <c r="B45" s="81"/>
+      <c r="C45" s="90"/>
       <c r="D45" s="28"/>
       <c r="E45" s="19"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="26"/>
-      <c r="B46" s="78"/>
-      <c r="C46" s="79"/>
+      <c r="B46" s="83"/>
+      <c r="C46" s="84"/>
       <c r="D46" s="29"/>
       <c r="E46" s="27"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="26"/>
-      <c r="B47" s="78"/>
-      <c r="C47" s="79"/>
+      <c r="B47" s="83"/>
+      <c r="C47" s="84"/>
       <c r="D47" s="29"/>
       <c r="E47" s="27"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="26"/>
-      <c r="B48" s="78"/>
-      <c r="C48" s="79"/>
+      <c r="B48" s="83"/>
+      <c r="C48" s="84"/>
       <c r="D48" s="29"/>
       <c r="E48" s="27"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="18"/>
-      <c r="B49" s="80"/>
-      <c r="C49" s="81"/>
+      <c r="B49" s="85"/>
+      <c r="C49" s="86"/>
       <c r="D49" s="30"/>
       <c r="E49" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="C14:E14"/>
@@ -1723,19 +1726,13 @@
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1750,10 +1747,10 @@
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="14" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
@@ -1814,17 +1811,17 @@
       <c r="E6" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="106" t="s">
+      <c r="F6" s="105" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="107"/>
+      <c r="G6" s="106"/>
       <c r="H6" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="98" t="s">
+      <c r="I6" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="99"/>
+      <c r="J6" s="98"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1839,15 +1836,15 @@
       <c r="E7" s="43">
         <v>1</v>
       </c>
-      <c r="F7" s="104" t="s">
+      <c r="F7" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="105"/>
+      <c r="G7" s="104"/>
       <c r="H7" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="100"/>
-      <c r="J7" s="101"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="100"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1863,15 +1860,15 @@
       <c r="E8" s="44">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F8" s="108" t="s">
+      <c r="F8" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="109"/>
+      <c r="G8" s="108"/>
       <c r="H8" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="100"/>
-      <c r="J8" s="101"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="100"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1887,15 +1884,15 @@
       <c r="E9" s="45">
         <v>1.2</v>
       </c>
-      <c r="F9" s="110" t="s">
+      <c r="F9" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="111"/>
+      <c r="G9" s="110"/>
       <c r="H9" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="100"/>
-      <c r="J9" s="101"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="100"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -1906,34 +1903,34 @@
       <c r="E10" s="45">
         <v>1.3</v>
       </c>
-      <c r="F10" s="110" t="s">
+      <c r="F10" s="109" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="111"/>
+      <c r="G10" s="110"/>
       <c r="H10" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="100"/>
-      <c r="J10" s="101"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="100"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="D11" s="40"/>
       <c r="E11" s="45"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="111"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="110"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="102"/>
-      <c r="J11" s="103"/>
+      <c r="I11" s="101"/>
+      <c r="J11" s="102"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="D12" s="40"/>
       <c r="E12" s="45"/>
-      <c r="F12" s="110"/>
-      <c r="G12" s="111"/>
+      <c r="F12" s="109"/>
+      <c r="G12" s="110"/>
       <c r="H12" s="47"/>
       <c r="I12" s="48"/>
     </row>
@@ -1942,8 +1939,8 @@
       <c r="B13" s="1"/>
       <c r="D13" s="40"/>
       <c r="E13" s="45"/>
-      <c r="F13" s="110"/>
-      <c r="G13" s="111"/>
+      <c r="F13" s="109"/>
+      <c r="G13" s="110"/>
       <c r="H13" s="47"/>
       <c r="I13" s="48"/>
     </row>
@@ -1952,16 +1949,16 @@
       <c r="B14" s="1"/>
       <c r="D14" s="40"/>
       <c r="E14" s="45"/>
-      <c r="F14" s="110"/>
-      <c r="G14" s="111"/>
+      <c r="F14" s="109"/>
+      <c r="G14" s="110"/>
       <c r="H14" s="11"/>
       <c r="I14" s="48"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" s="49"/>
       <c r="E15" s="46"/>
-      <c r="F15" s="96"/>
-      <c r="G15" s="97"/>
+      <c r="F15" s="95"/>
+      <c r="G15" s="96"/>
       <c r="H15" s="50"/>
     </row>
     <row r="16" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2022,7 +2019,7 @@
       </c>
       <c r="I18" s="61"/>
     </row>
-    <row r="19" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>10</v>
       </c>
@@ -2079,76 +2076,76 @@
       <c r="I20" s="22"/>
     </row>
     <row r="21" spans="1:10" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="67">
+      <c r="D21" s="66">
         <v>0</v>
       </c>
-      <c r="E21" s="68">
+      <c r="E21" s="67">
         <v>50</v>
       </c>
-      <c r="F21" s="69">
+      <c r="F21" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="62" t="s">
+      <c r="G21" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="H21" s="35" t="s">
+      <c r="H21" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="I21" s="70" t="s">
+      <c r="I21" s="69" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="35"/>
-      <c r="B22" s="71"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="69"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="68"/>
       <c r="E22" s="35"/>
-      <c r="F22" s="69">
+      <c r="F22" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="63"/>
+      <c r="G22" s="62"/>
       <c r="H22" s="35"/>
-      <c r="I22" s="72"/>
+      <c r="I22" s="71"/>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="35"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="69"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="68"/>
       <c r="E23" s="35"/>
-      <c r="F23" s="69">
+      <c r="F23" s="68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="63"/>
+      <c r="G23" s="62"/>
       <c r="H23" s="35"/>
-      <c r="I23" s="72"/>
+      <c r="I23" s="71"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="73"/>
-      <c r="B24" s="74"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="67">
+      <c r="A24" s="72"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="66">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="64"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="77"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="76"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>

</xml_diff>